<commit_message>
ta quase terminando sabosta
</commit_message>
<xml_diff>
--- a/PDCA.xlsx
+++ b/PDCA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tabler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tabler_Documentation\Tabler\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>P</t>
   </si>
@@ -78,6 +78,51 @@
   </si>
   <si>
     <t>Estruturar HTML para construção da página</t>
+  </si>
+  <si>
+    <t>Criação Banco de Dados</t>
+  </si>
+  <si>
+    <t>Definir quantidade de tabelas que serão necessárias para a aplicação</t>
+  </si>
+  <si>
+    <t>Criar tabelas com os campos definidos</t>
+  </si>
+  <si>
+    <t>Criar composição entre tabelas</t>
+  </si>
+  <si>
+    <t>Verificar se os dados estão sendo inseridos corretamente conforme definido os campos</t>
+  </si>
+  <si>
+    <t>Testar relacionamentos das tabelas</t>
+  </si>
+  <si>
+    <t>Verificar se os campos das tabelas estão no padrão definido pela equipe</t>
+  </si>
+  <si>
+    <t>Disponibilizar usuário e senha DBA para que o backend se conecte ao banco de dados</t>
+  </si>
+  <si>
+    <t>Criação de API para controle do chat</t>
+  </si>
+  <si>
+    <t>Procurar exemplos de chat criados em Golang</t>
+  </si>
+  <si>
+    <t>Estudar como cria este tipo de função utilizando a linguagem de programação Golang</t>
+  </si>
+  <si>
+    <t>Criar API para iniciar testes</t>
+  </si>
+  <si>
+    <t>Verificar se os dados estão sendo inseridos no BD</t>
+  </si>
+  <si>
+    <t>Criar versão final da API</t>
+  </si>
+  <si>
+    <t>Integrar API de chat com o frontend</t>
   </si>
 </sst>
 </file>
@@ -205,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -229,6 +274,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -517,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B15"/>
+      <selection activeCell="A26" sqref="A26:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,12 +674,126 @@
         <v>16</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="B22" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="B23" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
+      <c r="B29" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+      <c r="B31" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
+      <c r="B32" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A32"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A19:A20"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>